<commit_message>
Sync non-localized files for core commit 1a17ee8 Changes for core/source commit https://git.corp.adobe.com/AdobeDocs/experience-manager-cloud-service.en/commit/1a17ee86736b2d2bc868dbae40cb2a1ea99ca1ef
</commit_message>
<xml_diff>
--- a/help/edge/assets/enquiry.xlsx
+++ b/help/edge/assets/enquiry.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_F436F770082EBB28B5161DA7A14C6C5F419057BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7C82787-E8FD-4DDF-A802-F89F424637E8}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe.sharepoint.com/sites/wkndform/Shared Documents/wefinance1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="149" documentId="11_F436F770082EBB28B5161DA7A14C6C5F419057BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA3A3B2B-E715-41CD-BFA5-751F6D3308DA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="1060" windowWidth="15500" windowHeight="5900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="shared-default" sheetId="1" r:id="rId1"/>
+    <sheet name="shared-aem" sheetId="1" r:id="rId1"/>
     <sheet name="shared-country" sheetId="2" r:id="rId2"/>
     <sheet name="incoming" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="316">
   <si>
     <t>Name</t>
   </si>
@@ -119,87 +124,87 @@
     <t>Destination</t>
   </si>
   <si>
+    <t>https://main--wefinance--wkndform.aem.live/enquiry.json?sheet=country</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Please Select</t>
+  </si>
+  <si>
+    <t>Class of service</t>
+  </si>
+  <si>
+    <t>Economy, Business, First</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room Budget </t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Estimated Trip Cost</t>
+  </si>
+  <si>
+    <t>panel-1</t>
+  </si>
+  <si>
+    <t>fieldset</t>
+  </si>
+  <si>
+    <t>Traveler Info</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>subscribe</t>
+  </si>
+  <si>
+    <t>checkbox</t>
+  </si>
+  <si>
+    <t>Do you like subscribe for Magazine &amp; Activities?</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>Let's Talk</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
     <t>US</t>
   </si>
   <si>
-    <t>https://main--wefinance--wkndform.aem.live/enquiry.json?sheet=country</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>Please Select</t>
-  </si>
-  <si>
-    <t>Class of service</t>
-  </si>
-  <si>
-    <t>Economy, Business, First</t>
-  </si>
-  <si>
-    <t>budget</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room Budget </t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>Estimated Trip Cost</t>
-  </si>
-  <si>
-    <t>panel-1</t>
-  </si>
-  <si>
-    <t>fieldset</t>
-  </si>
-  <si>
-    <t>Traveler Info</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>subscribe</t>
-  </si>
-  <si>
-    <t>checkbox</t>
-  </si>
-  <si>
-    <t>Do you like subscribe for Magazine &amp; Activities?</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>submit</t>
-  </si>
-  <si>
-    <t>Let's Talk</t>
-  </si>
-  <si>
-    <t>Option</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>Afghanistan</t>
   </si>
   <si>
@@ -969,6 +974,18 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1030,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1024,6 +1041,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E1F2"/>
         <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDBDBD"/>
+        <bgColor rgb="FFBDBDBD"/>
       </patternFill>
     </fill>
   </fills>
@@ -1040,7 +1063,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1061,6 +1084,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1340,8 +1365,8 @@
   </sheetPr>
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1359,7 +1384,7 @@
     <col min="16384" max="16384" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75">
+    <row r="1" spans="1:25" ht="12.95">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1449,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" ht="12.75">
+    <row r="2" spans="1:25" ht="12.6">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -1456,7 +1481,7 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:25" ht="12.75">
+    <row r="3" spans="1:25" ht="12.6">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -1488,7 +1513,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:25" ht="12.75">
+    <row r="4" spans="1:25" ht="12.6">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1502,16 +1527,14 @@
         <v>27</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1524,18 +1547,18 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:25" ht="12.75">
+    <row r="5" spans="1:25" ht="12.6">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1545,7 +1568,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1558,22 +1581,24 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:25" ht="12.75">
+    <row r="6" spans="1:25" ht="12.6">
       <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="8">
         <v>1000</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" s="8">
         <v>500</v>
       </c>
@@ -1596,16 +1621,16 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:25" ht="12.75">
+    <row r="7" spans="1:25" ht="12.6">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="8"/>
@@ -1626,16 +1651,16 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="1:25" ht="12.75">
+    <row r="8" spans="1:25" ht="12.6">
       <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1643,7 +1668,9 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1656,12 +1683,12 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:25" ht="12.75">
+    <row r="9" spans="1:25" ht="12.6">
       <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
@@ -1673,7 +1700,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -1688,16 +1715,16 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:25" ht="12.75">
+    <row r="10" spans="1:25" ht="12.6">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1705,7 +1732,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -1720,16 +1747,16 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:25" ht="12.75">
+    <row r="11" spans="1:25" ht="12.6">
       <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="5" t="b">
@@ -1752,16 +1779,16 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:25" ht="12.75">
+    <row r="12" spans="1:25" ht="12.6">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1780,16 +1807,16 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:25" ht="12.75">
+    <row r="13" spans="1:25" ht="12.6">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1826,15 +1853,13 @@
   </sheetPr>
   <dimension ref="A1:Z241"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -1864,15 +1889,15 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>55</v>
       </c>
@@ -1880,7 +1905,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>56</v>
       </c>
@@ -1888,7 +1913,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>57</v>
       </c>
@@ -1896,7 +1921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>58</v>
       </c>
@@ -1904,7 +1929,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>59</v>
       </c>
@@ -1912,7 +1937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>60</v>
       </c>
@@ -1920,7 +1945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>61</v>
       </c>
@@ -1928,7 +1953,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>62</v>
       </c>
@@ -1936,7 +1961,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>63</v>
       </c>
@@ -1944,7 +1969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
@@ -1952,7 +1977,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>66</v>
       </c>
@@ -1960,7 +1985,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>67</v>
       </c>
@@ -1968,7 +1993,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>68</v>
       </c>
@@ -1976,7 +2001,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>69</v>
       </c>
@@ -1984,7 +2009,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>70</v>
       </c>
@@ -1992,7 +2017,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>71</v>
       </c>
@@ -2000,7 +2025,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>72</v>
       </c>
@@ -2008,7 +2033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>73</v>
       </c>
@@ -2016,7 +2041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="14.45">
       <c r="A21" s="10" t="s">
         <v>74</v>
       </c>
@@ -2024,7 +2049,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="14.45">
       <c r="A22" s="9" t="s">
         <v>75</v>
       </c>
@@ -2032,7 +2057,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="14.45">
       <c r="A23" s="10" t="s">
         <v>76</v>
       </c>
@@ -2040,7 +2065,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="14.45">
       <c r="A24" s="9" t="s">
         <v>77</v>
       </c>
@@ -2048,7 +2073,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="14.45">
       <c r="A25" s="10" t="s">
         <v>78</v>
       </c>
@@ -2056,7 +2081,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" ht="14.45">
       <c r="A26" s="9" t="s">
         <v>79</v>
       </c>
@@ -2064,7 +2089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="14.45">
       <c r="A27" s="10" t="s">
         <v>80</v>
       </c>
@@ -2072,7 +2097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" ht="14.45">
       <c r="A28" s="9" t="s">
         <v>81</v>
       </c>
@@ -2080,7 +2105,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" ht="14.45">
       <c r="A29" s="10" t="s">
         <v>82</v>
       </c>
@@ -2088,7 +2113,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" ht="14.45">
       <c r="A30" s="9" t="s">
         <v>83</v>
       </c>
@@ -2096,7 +2121,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" ht="14.45">
       <c r="A31" s="10" t="s">
         <v>84</v>
       </c>
@@ -2104,7 +2129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" ht="14.45">
       <c r="A32" s="9" t="s">
         <v>85</v>
       </c>
@@ -2112,7 +2137,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" ht="14.45">
       <c r="A33" s="10" t="s">
         <v>86</v>
       </c>
@@ -2120,7 +2145,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" ht="14.45">
       <c r="A34" s="9" t="s">
         <v>88</v>
       </c>
@@ -2128,7 +2153,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" ht="14.45">
       <c r="A35" s="10" t="s">
         <v>89</v>
       </c>
@@ -2136,7 +2161,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" ht="14.45">
       <c r="A36" s="9" t="s">
         <v>90</v>
       </c>
@@ -2144,7 +2169,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" ht="14.45">
       <c r="A37" s="10" t="s">
         <v>91</v>
       </c>
@@ -2152,7 +2177,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" ht="14.45">
       <c r="A38" s="9" t="s">
         <v>92</v>
       </c>
@@ -2160,7 +2185,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" ht="14.45">
       <c r="A39" s="10" t="s">
         <v>93</v>
       </c>
@@ -2168,7 +2193,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" ht="14.45">
       <c r="A40" s="9" t="s">
         <v>94</v>
       </c>
@@ -2176,7 +2201,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" ht="14.45">
       <c r="A41" s="10" t="s">
         <v>95</v>
       </c>
@@ -2184,7 +2209,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" ht="14.45">
       <c r="A42" s="9" t="s">
         <v>97</v>
       </c>
@@ -2192,7 +2217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" ht="14.45">
       <c r="A43" s="10" t="s">
         <v>98</v>
       </c>
@@ -2200,7 +2225,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" ht="14.45">
       <c r="A44" s="9" t="s">
         <v>99</v>
       </c>
@@ -2208,7 +2233,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" ht="14.45">
       <c r="A45" s="10" t="s">
         <v>100</v>
       </c>
@@ -2216,7 +2241,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" ht="14.45">
       <c r="A46" s="9" t="s">
         <v>101</v>
       </c>
@@ -2224,7 +2249,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" ht="14.45">
       <c r="A47" s="10" t="s">
         <v>103</v>
       </c>
@@ -2232,7 +2257,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" ht="14.45">
       <c r="A48" s="9" t="s">
         <v>105</v>
       </c>
@@ -2240,7 +2265,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" ht="14.45">
       <c r="A49" s="10" t="s">
         <v>106</v>
       </c>
@@ -2248,7 +2273,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" ht="14.45">
       <c r="A50" s="9" t="s">
         <v>107</v>
       </c>
@@ -2256,7 +2281,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" ht="14.45">
       <c r="A51" s="10" t="s">
         <v>108</v>
       </c>
@@ -2264,7 +2289,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" ht="14.45">
       <c r="A52" s="9" t="s">
         <v>110</v>
       </c>
@@ -2272,7 +2297,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" ht="14.45">
       <c r="A53" s="10" t="s">
         <v>111</v>
       </c>
@@ -2280,7 +2305,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" ht="14.45">
       <c r="A54" s="9" t="s">
         <v>112</v>
       </c>
@@ -2288,7 +2313,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" ht="14.45">
       <c r="A55" s="10" t="s">
         <v>113</v>
       </c>
@@ -2296,7 +2321,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" ht="14.45">
       <c r="A56" s="9" t="s">
         <v>114</v>
       </c>
@@ -2304,7 +2329,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" ht="14.45">
       <c r="A57" s="10" t="s">
         <v>115</v>
       </c>
@@ -2312,7 +2337,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" ht="14.45">
       <c r="A58" s="9" t="s">
         <v>116</v>
       </c>
@@ -2320,7 +2345,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" ht="14.45">
       <c r="A59" s="10" t="s">
         <v>117</v>
       </c>
@@ -2328,7 +2353,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" ht="14.45">
       <c r="A60" s="9" t="s">
         <v>118</v>
       </c>
@@ -2336,7 +2361,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" ht="14.45">
       <c r="A61" s="10" t="s">
         <v>119</v>
       </c>
@@ -2344,7 +2369,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" ht="14.45">
       <c r="A62" s="9" t="s">
         <v>120</v>
       </c>
@@ -2352,7 +2377,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" ht="14.45">
       <c r="A63" s="10" t="s">
         <v>121</v>
       </c>
@@ -2360,7 +2385,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" ht="14.45">
       <c r="A64" s="9" t="s">
         <v>122</v>
       </c>
@@ -2368,7 +2393,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" ht="14.45">
       <c r="A65" s="10" t="s">
         <v>123</v>
       </c>
@@ -2376,7 +2401,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" ht="14.45">
       <c r="A66" s="9" t="s">
         <v>124</v>
       </c>
@@ -2384,7 +2409,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" ht="14.45">
       <c r="A67" s="10" t="s">
         <v>125</v>
       </c>
@@ -2392,7 +2417,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" ht="14.45">
       <c r="A68" s="9" t="s">
         <v>127</v>
       </c>
@@ -2400,7 +2425,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" ht="14.45">
       <c r="A69" s="10" t="s">
         <v>128</v>
       </c>
@@ -2408,7 +2433,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" ht="14.45">
       <c r="A70" s="9" t="s">
         <v>129</v>
       </c>
@@ -2416,7 +2441,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" ht="14.45">
       <c r="A71" s="10" t="s">
         <v>130</v>
       </c>
@@ -2424,7 +2449,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" ht="14.45">
       <c r="A72" s="9" t="s">
         <v>131</v>
       </c>
@@ -2432,7 +2457,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" ht="14.45">
       <c r="A73" s="10" t="s">
         <v>132</v>
       </c>
@@ -2440,7 +2465,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" ht="14.45">
       <c r="A74" s="9" t="s">
         <v>133</v>
       </c>
@@ -2448,7 +2473,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" ht="14.45">
       <c r="A75" s="10" t="s">
         <v>134</v>
       </c>
@@ -2456,7 +2481,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" ht="14.45">
       <c r="A76" s="9" t="s">
         <v>135</v>
       </c>
@@ -2464,7 +2489,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" ht="14.45">
       <c r="A77" s="10" t="s">
         <v>136</v>
       </c>
@@ -2472,7 +2497,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" ht="14.45">
       <c r="A78" s="9" t="s">
         <v>137</v>
       </c>
@@ -2480,7 +2505,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" ht="14.45">
       <c r="A79" s="10" t="s">
         <v>139</v>
       </c>
@@ -2488,7 +2513,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" ht="14.45">
       <c r="A80" s="9" t="s">
         <v>140</v>
       </c>
@@ -2496,7 +2521,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" ht="14.45">
       <c r="A81" s="10" t="s">
         <v>141</v>
       </c>
@@ -2504,7 +2529,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" ht="14.45">
       <c r="A82" s="9" t="s">
         <v>142</v>
       </c>
@@ -2512,7 +2537,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" ht="14.45">
       <c r="A83" s="10" t="s">
         <v>143</v>
       </c>
@@ -2520,7 +2545,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" ht="14.45">
       <c r="A84" s="9" t="s">
         <v>144</v>
       </c>
@@ -2528,7 +2553,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" ht="14.45">
       <c r="A85" s="10" t="s">
         <v>145</v>
       </c>
@@ -2536,7 +2561,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" ht="14.45">
       <c r="A86" s="9" t="s">
         <v>147</v>
       </c>
@@ -2544,7 +2569,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" ht="14.45">
       <c r="A87" s="10" t="s">
         <v>148</v>
       </c>
@@ -2552,7 +2577,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" ht="14.45">
       <c r="A88" s="9" t="s">
         <v>149</v>
       </c>
@@ -2560,7 +2585,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" ht="14.45">
       <c r="A89" s="10" t="s">
         <v>150</v>
       </c>
@@ -2568,7 +2593,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" ht="14.45">
       <c r="A90" s="9" t="s">
         <v>151</v>
       </c>
@@ -2576,7 +2601,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" ht="14.45">
       <c r="A91" s="10" t="s">
         <v>152</v>
       </c>
@@ -2584,7 +2609,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" ht="14.45">
       <c r="A92" s="9" t="s">
         <v>153</v>
       </c>
@@ -2592,7 +2617,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" ht="14.45">
       <c r="A93" s="10" t="s">
         <v>154</v>
       </c>
@@ -2600,7 +2625,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" ht="14.45">
       <c r="A94" s="9" t="s">
         <v>156</v>
       </c>
@@ -2608,7 +2633,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" ht="14.45">
       <c r="A95" s="10" t="s">
         <v>157</v>
       </c>
@@ -2616,7 +2641,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" ht="14.45">
       <c r="A96" s="9" t="s">
         <v>158</v>
       </c>
@@ -2624,7 +2649,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" ht="14.45">
       <c r="A97" s="10" t="s">
         <v>159</v>
       </c>
@@ -2632,7 +2657,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" ht="14.45">
       <c r="A98" s="9" t="s">
         <v>160</v>
       </c>
@@ -2640,7 +2665,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" ht="14.45">
       <c r="A99" s="10" t="s">
         <v>161</v>
       </c>
@@ -2648,7 +2673,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" ht="14.45">
       <c r="A100" s="9" t="s">
         <v>162</v>
       </c>
@@ -2656,7 +2681,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" ht="14.45">
       <c r="A101" s="10" t="s">
         <v>163</v>
       </c>
@@ -2664,7 +2689,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" ht="14.45">
       <c r="A102" s="9" t="s">
         <v>164</v>
       </c>
@@ -2672,7 +2697,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" ht="14.45">
       <c r="A103" s="10" t="s">
         <v>165</v>
       </c>
@@ -2680,7 +2705,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" ht="14.45">
       <c r="A104" s="9" t="s">
         <v>166</v>
       </c>
@@ -2688,7 +2713,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" ht="14.45">
       <c r="A105" s="10" t="s">
         <v>167</v>
       </c>
@@ -2696,7 +2721,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" ht="14.45">
       <c r="A106" s="9" t="s">
         <v>168</v>
       </c>
@@ -2704,7 +2729,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" ht="14.45">
       <c r="A107" s="10" t="s">
         <v>169</v>
       </c>
@@ -2712,7 +2737,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" ht="14.45">
       <c r="A108" s="9" t="s">
         <v>170</v>
       </c>
@@ -2720,7 +2745,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" ht="14.45">
       <c r="A109" s="10" t="s">
         <v>171</v>
       </c>
@@ -2728,7 +2753,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" ht="14.45">
       <c r="A110" s="9" t="s">
         <v>172</v>
       </c>
@@ -2736,7 +2761,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" ht="14.45">
       <c r="A111" s="10" t="s">
         <v>173</v>
       </c>
@@ -2744,7 +2769,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" ht="14.45">
       <c r="A112" s="9" t="s">
         <v>175</v>
       </c>
@@ -2752,7 +2777,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" ht="14.45">
       <c r="A113" s="10" t="s">
         <v>176</v>
       </c>
@@ -2760,7 +2785,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" ht="14.45">
       <c r="A114" s="9" t="s">
         <v>178</v>
       </c>
@@ -2768,7 +2793,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" ht="14.45">
       <c r="A115" s="10" t="s">
         <v>179</v>
       </c>
@@ -2776,7 +2801,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" ht="14.45">
       <c r="A116" s="9" t="s">
         <v>180</v>
       </c>
@@ -2784,7 +2809,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" ht="14.45">
       <c r="A117" s="10" t="s">
         <v>181</v>
       </c>
@@ -2792,7 +2817,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" ht="14.45">
       <c r="A118" s="9" t="s">
         <v>182</v>
       </c>
@@ -2800,7 +2825,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" ht="14.45">
       <c r="A119" s="10" t="s">
         <v>183</v>
       </c>
@@ -2808,7 +2833,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" ht="14.45">
       <c r="A120" s="9" t="s">
         <v>184</v>
       </c>
@@ -2816,7 +2841,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" ht="14.45">
       <c r="A121" s="10" t="s">
         <v>186</v>
       </c>
@@ -2824,7 +2849,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" ht="14.45">
       <c r="A122" s="9" t="s">
         <v>187</v>
       </c>
@@ -2832,7 +2857,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" ht="14.45">
       <c r="A123" s="10" t="s">
         <v>188</v>
       </c>
@@ -2840,7 +2865,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" ht="14.45">
       <c r="A124" s="9" t="s">
         <v>189</v>
       </c>
@@ -2848,7 +2873,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" ht="14.45">
       <c r="A125" s="10" t="s">
         <v>190</v>
       </c>
@@ -2856,7 +2881,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" ht="14.45">
       <c r="A126" s="9" t="s">
         <v>191</v>
       </c>
@@ -2864,7 +2889,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" ht="14.45">
       <c r="A127" s="10" t="s">
         <v>192</v>
       </c>
@@ -2872,7 +2897,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" ht="14.45">
       <c r="A128" s="9" t="s">
         <v>193</v>
       </c>
@@ -2880,7 +2905,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" ht="14.45">
       <c r="A129" s="10" t="s">
         <v>194</v>
       </c>
@@ -2888,7 +2913,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" ht="14.45">
       <c r="A130" s="9" t="s">
         <v>195</v>
       </c>
@@ -2896,7 +2921,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" ht="14.45">
       <c r="A131" s="10" t="s">
         <v>196</v>
       </c>
@@ -2904,7 +2929,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" ht="14.45">
       <c r="A132" s="9" t="s">
         <v>197</v>
       </c>
@@ -2912,7 +2937,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" ht="14.45">
       <c r="A133" s="10" t="s">
         <v>198</v>
       </c>
@@ -2920,7 +2945,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" ht="14.45">
       <c r="A134" s="9" t="s">
         <v>199</v>
       </c>
@@ -2928,7 +2953,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" ht="14.45">
       <c r="A135" s="10" t="s">
         <v>200</v>
       </c>
@@ -2936,7 +2961,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" ht="14.45">
       <c r="A136" s="9" t="s">
         <v>201</v>
       </c>
@@ -2944,7 +2969,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" ht="14.45">
       <c r="A137" s="10" t="s">
         <v>202</v>
       </c>
@@ -2952,7 +2977,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" ht="14.45">
       <c r="A138" s="9" t="s">
         <v>203</v>
       </c>
@@ -2960,7 +2985,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" ht="14.45">
       <c r="A139" s="10" t="s">
         <v>204</v>
       </c>
@@ -2968,7 +2993,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" ht="14.45">
       <c r="A140" s="9" t="s">
         <v>205</v>
       </c>
@@ -2976,7 +3001,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" ht="14.45">
       <c r="A141" s="10" t="s">
         <v>206</v>
       </c>
@@ -2984,7 +3009,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" ht="14.45">
       <c r="A142" s="9" t="s">
         <v>207</v>
       </c>
@@ -2992,7 +3017,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" ht="14.45">
       <c r="A143" s="10" t="s">
         <v>208</v>
       </c>
@@ -3000,7 +3025,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" ht="14.45">
       <c r="A144" s="9" t="s">
         <v>209</v>
       </c>
@@ -3008,7 +3033,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" ht="14.45">
       <c r="A145" s="10" t="s">
         <v>211</v>
       </c>
@@ -3016,7 +3041,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" ht="14.45">
       <c r="A146" s="9" t="s">
         <v>212</v>
       </c>
@@ -3024,7 +3049,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" ht="14.45">
       <c r="A147" s="10" t="s">
         <v>213</v>
       </c>
@@ -3032,7 +3057,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" ht="14.45">
       <c r="A148" s="9" t="s">
         <v>214</v>
       </c>
@@ -3040,7 +3065,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" ht="14.45">
       <c r="A149" s="10" t="s">
         <v>215</v>
       </c>
@@ -3048,7 +3073,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" ht="14.45">
       <c r="A150" s="9" t="s">
         <v>216</v>
       </c>
@@ -3056,7 +3081,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" ht="14.45">
       <c r="A151" s="10" t="s">
         <v>217</v>
       </c>
@@ -3064,7 +3089,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" ht="14.45">
       <c r="A152" s="9" t="s">
         <v>218</v>
       </c>
@@ -3072,7 +3097,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" ht="14.45">
       <c r="A153" s="10" t="s">
         <v>219</v>
       </c>
@@ -3080,7 +3105,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" ht="14.45">
       <c r="A154" s="9" t="s">
         <v>220</v>
       </c>
@@ -3088,7 +3113,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" ht="14.45">
       <c r="A155" s="10" t="s">
         <v>221</v>
       </c>
@@ -3096,7 +3121,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" ht="14.45">
       <c r="A156" s="9" t="s">
         <v>222</v>
       </c>
@@ -3104,7 +3129,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" ht="14.45">
       <c r="A157" s="10" t="s">
         <v>223</v>
       </c>
@@ -3112,7 +3137,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" ht="14.45">
       <c r="A158" s="9" t="s">
         <v>224</v>
       </c>
@@ -3120,7 +3145,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" ht="14.45">
       <c r="A159" s="10" t="s">
         <v>225</v>
       </c>
@@ -3128,7 +3153,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" ht="14.45">
       <c r="A160" s="9" t="s">
         <v>226</v>
       </c>
@@ -3136,7 +3161,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" ht="14.45">
       <c r="A161" s="10" t="s">
         <v>227</v>
       </c>
@@ -3144,7 +3169,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" ht="14.45">
       <c r="A162" s="9" t="s">
         <v>228</v>
       </c>
@@ -3152,7 +3177,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" ht="14.45">
       <c r="A163" s="10" t="s">
         <v>229</v>
       </c>
@@ -3160,7 +3185,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" ht="14.45">
       <c r="A164" s="9" t="s">
         <v>230</v>
       </c>
@@ -3168,7 +3193,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" ht="14.45">
       <c r="A165" s="10" t="s">
         <v>231</v>
       </c>
@@ -3176,7 +3201,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" ht="14.45">
       <c r="A166" s="9" t="s">
         <v>232</v>
       </c>
@@ -3184,7 +3209,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" ht="14.45">
       <c r="A167" s="10" t="s">
         <v>233</v>
       </c>
@@ -3192,7 +3217,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" ht="14.45">
       <c r="A168" s="9" t="s">
         <v>234</v>
       </c>
@@ -3200,7 +3225,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" ht="14.45">
       <c r="A169" s="10" t="s">
         <v>236</v>
       </c>
@@ -3208,7 +3233,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" ht="14.45">
       <c r="A170" s="9" t="s">
         <v>237</v>
       </c>
@@ -3216,7 +3241,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" ht="14.45">
       <c r="A171" s="10" t="s">
         <v>238</v>
       </c>
@@ -3224,7 +3249,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" ht="14.45">
       <c r="A172" s="9" t="s">
         <v>240</v>
       </c>
@@ -3232,7 +3257,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" ht="14.45">
       <c r="A173" s="10" t="s">
         <v>241</v>
       </c>
@@ -3240,7 +3265,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" ht="14.45">
       <c r="A174" s="9" t="s">
         <v>242</v>
       </c>
@@ -3248,7 +3273,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" ht="14.45">
       <c r="A175" s="10" t="s">
         <v>244</v>
       </c>
@@ -3256,7 +3281,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" ht="14.45">
       <c r="A176" s="9" t="s">
         <v>245</v>
       </c>
@@ -3264,7 +3289,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" ht="14.45">
       <c r="A177" s="10" t="s">
         <v>246</v>
       </c>
@@ -3272,7 +3297,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" ht="14.45">
       <c r="A178" s="9" t="s">
         <v>247</v>
       </c>
@@ -3280,7 +3305,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" ht="14.45">
       <c r="A179" s="10" t="s">
         <v>248</v>
       </c>
@@ -3288,7 +3313,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" ht="14.45">
       <c r="A180" s="9" t="s">
         <v>249</v>
       </c>
@@ -3296,7 +3321,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" ht="14.45">
       <c r="A181" s="10" t="s">
         <v>250</v>
       </c>
@@ -3304,7 +3329,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" ht="14.45">
       <c r="A182" s="9" t="s">
         <v>251</v>
       </c>
@@ -3312,7 +3337,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" ht="14.45">
       <c r="A183" s="10" t="s">
         <v>252</v>
       </c>
@@ -3320,7 +3345,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" ht="14.45">
       <c r="A184" s="9" t="s">
         <v>253</v>
       </c>
@@ -3328,7 +3353,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" ht="14.45">
       <c r="A185" s="10" t="s">
         <v>254</v>
       </c>
@@ -3336,7 +3361,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" ht="14.45">
       <c r="A186" s="9" t="s">
         <v>255</v>
       </c>
@@ -3344,7 +3369,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" ht="14.45">
       <c r="A187" s="10" t="s">
         <v>256</v>
       </c>
@@ -3352,7 +3377,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" ht="14.45">
       <c r="A188" s="9" t="s">
         <v>257</v>
       </c>
@@ -3360,7 +3385,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" ht="14.45">
       <c r="A189" s="10" t="s">
         <v>258</v>
       </c>
@@ -3368,7 +3393,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" ht="14.45">
       <c r="A190" s="9" t="s">
         <v>259</v>
       </c>
@@ -3376,7 +3401,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" ht="14.45">
       <c r="A191" s="10" t="s">
         <v>260</v>
       </c>
@@ -3384,7 +3409,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" ht="14.45">
       <c r="A192" s="9" t="s">
         <v>261</v>
       </c>
@@ -3392,7 +3417,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" ht="14.45">
       <c r="A193" s="10" t="s">
         <v>262</v>
       </c>
@@ -3400,7 +3425,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" ht="14.45">
       <c r="A194" s="9" t="s">
         <v>263</v>
       </c>
@@ -3408,7 +3433,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" ht="14.45">
       <c r="A195" s="10" t="s">
         <v>264</v>
       </c>
@@ -3416,7 +3441,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" ht="14.45">
       <c r="A196" s="9" t="s">
         <v>265</v>
       </c>
@@ -3424,7 +3449,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" ht="14.45">
       <c r="A197" s="10" t="s">
         <v>266</v>
       </c>
@@ -3432,7 +3457,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" ht="14.45">
       <c r="A198" s="9" t="s">
         <v>267</v>
       </c>
@@ -3440,7 +3465,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" ht="14.45">
       <c r="A199" s="10" t="s">
         <v>268</v>
       </c>
@@ -3448,7 +3473,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" ht="14.45">
       <c r="A200" s="9" t="s">
         <v>269</v>
       </c>
@@ -3456,7 +3481,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" ht="14.45">
       <c r="A201" s="10" t="s">
         <v>270</v>
       </c>
@@ -3464,7 +3489,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" ht="14.45">
       <c r="A202" s="9" t="s">
         <v>271</v>
       </c>
@@ -3472,7 +3497,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" ht="14.45">
       <c r="A203" s="10" t="s">
         <v>272</v>
       </c>
@@ -3480,7 +3505,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" ht="14.45">
       <c r="A204" s="9" t="s">
         <v>273</v>
       </c>
@@ -3488,7 +3513,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" ht="14.45">
       <c r="A205" s="10" t="s">
         <v>274</v>
       </c>
@@ -3496,7 +3521,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" ht="14.45">
       <c r="A206" s="9" t="s">
         <v>275</v>
       </c>
@@ -3504,7 +3529,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" ht="14.45">
       <c r="A207" s="10" t="s">
         <v>276</v>
       </c>
@@ -3512,7 +3537,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" ht="14.45">
       <c r="A208" s="9" t="s">
         <v>277</v>
       </c>
@@ -3520,7 +3545,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" ht="14.45">
       <c r="A209" s="10" t="s">
         <v>278</v>
       </c>
@@ -3528,7 +3553,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" ht="14.45">
       <c r="A210" s="9" t="s">
         <v>279</v>
       </c>
@@ -3536,7 +3561,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" ht="14.45">
       <c r="A211" s="10" t="s">
         <v>280</v>
       </c>
@@ -3544,7 +3569,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" ht="14.45">
       <c r="A212" s="9" t="s">
         <v>281</v>
       </c>
@@ -3552,7 +3577,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" ht="14.45">
       <c r="A213" s="10" t="s">
         <v>282</v>
       </c>
@@ -3560,7 +3585,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" ht="14.45">
       <c r="A214" s="9" t="s">
         <v>283</v>
       </c>
@@ -3568,7 +3593,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" ht="14.45">
       <c r="A215" s="10" t="s">
         <v>284</v>
       </c>
@@ -3576,7 +3601,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" ht="14.45">
       <c r="A216" s="9" t="s">
         <v>285</v>
       </c>
@@ -3584,7 +3609,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" ht="14.45">
       <c r="A217" s="10" t="s">
         <v>286</v>
       </c>
@@ -3592,7 +3617,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" ht="14.45">
       <c r="A218" s="9" t="s">
         <v>287</v>
       </c>
@@ -3600,7 +3625,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" ht="14.45">
       <c r="A219" s="10" t="s">
         <v>288</v>
       </c>
@@ -3608,7 +3633,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" ht="14.45">
       <c r="A220" s="9" t="s">
         <v>289</v>
       </c>
@@ -3616,7 +3641,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" ht="14.45">
       <c r="A221" s="10" t="s">
         <v>290</v>
       </c>
@@ -3624,7 +3649,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" ht="14.45">
       <c r="A222" s="9" t="s">
         <v>291</v>
       </c>
@@ -3632,7 +3657,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" ht="14.45">
       <c r="A223" s="10" t="s">
         <v>292</v>
       </c>
@@ -3640,7 +3665,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" ht="14.45">
       <c r="A224" s="9" t="s">
         <v>293</v>
       </c>
@@ -3648,7 +3673,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" ht="14.45">
       <c r="A225" s="10" t="s">
         <v>294</v>
       </c>
@@ -3656,7 +3681,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" ht="14.45">
       <c r="A226" s="9" t="s">
         <v>295</v>
       </c>
@@ -3664,7 +3689,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" ht="14.45">
       <c r="A227" s="10" t="s">
         <v>296</v>
       </c>
@@ -3672,7 +3697,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" ht="14.45">
       <c r="A228" s="9" t="s">
         <v>297</v>
       </c>
@@ -3680,7 +3705,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" ht="14.45">
       <c r="A229" s="10" t="s">
         <v>298</v>
       </c>
@@ -3688,7 +3713,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" ht="14.45">
       <c r="A230" s="9" t="s">
         <v>299</v>
       </c>
@@ -3696,7 +3721,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" ht="14.45">
       <c r="A231" s="10" t="s">
         <v>301</v>
       </c>
@@ -3704,7 +3729,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" ht="14.45">
       <c r="A232" s="9" t="s">
         <v>302</v>
       </c>
@@ -3712,7 +3737,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" ht="14.45">
       <c r="A233" s="10" t="s">
         <v>303</v>
       </c>
@@ -3720,7 +3745,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" ht="14.45">
       <c r="A234" s="9" t="s">
         <v>304</v>
       </c>
@@ -3728,7 +3753,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" ht="14.45">
       <c r="A235" s="10" t="s">
         <v>305</v>
       </c>
@@ -3736,7 +3761,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" ht="14.45">
       <c r="A236" s="9" t="s">
         <v>306</v>
       </c>
@@ -3744,7 +3769,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" ht="14.45">
       <c r="A237" s="10" t="s">
         <v>307</v>
       </c>
@@ -3752,7 +3777,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" ht="14.45">
       <c r="A238" s="9" t="s">
         <v>308</v>
       </c>
@@ -3760,7 +3785,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" ht="14.45">
       <c r="A239" s="10" t="s">
         <v>309</v>
       </c>
@@ -3768,7 +3793,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" ht="14.45">
       <c r="A240" s="9" t="s">
         <v>310</v>
       </c>
@@ -3776,7 +3801,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" ht="14.45">
       <c r="A241" s="10" t="s">
         <v>311</v>
       </c>
@@ -3796,57 +3821,104 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="D1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A2" s="12">
+        <v>45726</v>
+      </c>
+      <c r="B2" s="12">
+        <v>45731</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E2">
+        <v>1500000</v>
+      </c>
+      <c r="F2">
+        <v>15000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>314</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="3"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{1DF75BD8-07D4-4C66-A323-E8C3C235A20D}"/>
+  </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D18776F3B0E0D042A986A9831F3901DD" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d96493bbe2b936703aaac5c5bb600b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e1104a56-86c2-4cfe-a749-0b0a179bd022" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e873557fbfb0414b9f2c747667c66054" ns2:_="">
     <xsd:import namespace="e1104a56-86c2-4cfe-a749-0b0a179bd022"/>
@@ -3990,15 +4062,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4006,11 +4069,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF45CAF5-38C5-422A-8156-4B6E822C4490}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAFC511-D82D-4870-ABFE-90AAC1CBA552}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAFC511-D82D-4870-ABFE-90AAC1CBA552}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF45CAF5-38C5-422A-8156-4B6E822C4490}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>